<commit_message>
add outliers handling for continuous metrics
</commit_message>
<xml_diff>
--- a/src/example.xlsx
+++ b/src/example.xlsx
@@ -483,7 +483,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Unique ids: 6</t>
+          <t>Unique ids: 9</t>
         </is>
       </c>
     </row>
@@ -543,12 +543,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>33.33%</t>
+          <t>50.00%</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>50.00%</t>
+          <t>40.00%</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -558,19 +558,19 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>+50.00%</t>
+          <t>-20.00%</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>+200.00%</t>
+          <t>+100.00%</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>0.7641771556220945</v>
       </c>
       <c r="H11" t="n">
-        <v>0.992852315959681</v>
+        <v>0.4413427238396865</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
@@ -587,40 +587,40 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>162.50%</t>
+          <t>76.00%</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>127.27%</t>
+          <t>113.64%</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>250.00%</t>
+          <t>104.76%</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>-21.68%</t>
+          <t>+49.52%</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>+53.85%</t>
+          <t>+37.84%</t>
         </is>
       </c>
       <c r="G12" t="n">
+        <v>5.551375349886539e-07</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.005393233202449595</v>
+      </c>
+      <c r="I12" t="b">
         <v>1</v>
       </c>
-      <c r="H12" t="n">
+      <c r="J12" t="b">
         <v>1</v>
-      </c>
-      <c r="I12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -668,7 +668,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.6592430036926306</v>
+        <v>0.7641771556220945</v>
       </c>
       <c r="D17" t="n">
         <v>0.05</v>
@@ -677,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>0.7641771556220945</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -691,7 +691,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.2482130789899203</v>
+        <v>0.2206713619198432</v>
       </c>
       <c r="D18" t="n">
         <v>0.05</v>
@@ -700,7 +700,7 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.992852315959681</v>
+        <v>0.4413427238396865</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -718,19 +718,19 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>1.387843837471635e-07</v>
       </c>
       <c r="D19" t="n">
         <v>0.05</v>
       </c>
       <c r="E19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
+        <v>5.551375349886539e-07</v>
+      </c>
+      <c r="G19" t="n">
         <v>1</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -741,19 +741,19 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>0.001797744400816532</v>
       </c>
       <c r="D20" t="n">
         <v>0.05</v>
       </c>
       <c r="E20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
+        <v>0.005393233202449595</v>
+      </c>
+      <c r="G20" t="n">
         <v>1</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -806,7 +806,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Unique ids: 6</t>
+          <t>Unique ids: 9</t>
         </is>
       </c>
     </row>
@@ -961,7 +961,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -996,7 +996,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Unique ids: 6</t>
+          <t>Unique ids: 9</t>
         </is>
       </c>
     </row>
@@ -1054,81 +1054,114 @@
           <t>ARPU (USD after fee)</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>110.000</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>110.000</t>
+          <t>210.000</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>130.000</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+          <t>145.000</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>+90.91%</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>+31.82%</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>metric</t>
-        </is>
-      </c>
-      <c r="B15" s="1" t="inlineStr"/>
-      <c r="C15" s="1" t="inlineStr">
-        <is>
-          <t>pvalue</t>
-        </is>
-      </c>
-      <c r="D15" s="1" t="inlineStr">
-        <is>
-          <t>sig_level</t>
-        </is>
-      </c>
-      <c r="E15" s="1" t="inlineStr">
-        <is>
-          <t>significance</t>
-        </is>
-      </c>
-      <c r="F15" s="1" t="inlineStr">
-        <is>
-          <t>corrected_pvalue</t>
-        </is>
-      </c>
-      <c r="G15" s="1" t="inlineStr">
-        <is>
-          <t>corrected_significance</t>
-        </is>
-      </c>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>ARPU (USD after fee) - quantile 0.98</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>110.000</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>210.000</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>15.000</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>+90.91%</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-86.36%</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
+          <t>metric</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr"/>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>pvalue</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="inlineStr">
+        <is>
+          <t>sig_level</t>
+        </is>
+      </c>
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>significance</t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="inlineStr">
+        <is>
+          <t>corrected_pvalue</t>
+        </is>
+      </c>
+      <c r="G16" s="1" t="inlineStr">
+        <is>
+          <t>corrected_significance</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
           <t>ARPU (USD after fee)</t>
         </is>
       </c>
-      <c r="B16" s="1" t="inlineStr">
+      <c r="B17" s="1" t="inlineStr">
         <is>
           <t>2-1</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n"/>
-      <c r="B17" s="1" t="inlineStr">
-        <is>
-          <t>3-1</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -1139,9 +1172,59 @@
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
     </row>
+    <row r="18">
+      <c r="A18" s="1" t="n"/>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>3-1</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>ARPU (USD after fee) - quantile 0.98</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>2-1</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n"/>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>3-1</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A16:A17"/>
+  <mergeCells count="2">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix empty data to calc pvalue
</commit_message>
<xml_diff>
--- a/src/example.xlsx
+++ b/src/example.xlsx
@@ -679,7 +679,7 @@
       <c r="F17" t="n">
         <v>0.7641771556220945</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G17" t="b">
         <v>0</v>
       </c>
     </row>
@@ -702,7 +702,7 @@
       <c r="F18" t="n">
         <v>0.4413427238396865</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G18" t="b">
         <v>0</v>
       </c>
     </row>
@@ -729,7 +729,7 @@
       <c r="F19" t="n">
         <v>5.551375349886539e-07</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G19" t="b">
         <v>1</v>
       </c>
     </row>
@@ -752,7 +752,7 @@
       <c r="F20" t="n">
         <v>0.005393233202449595</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20" t="b">
         <v>1</v>
       </c>
     </row>
@@ -771,7 +771,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -946,11 +946,29 @@
       <c r="F16" t="n">
         <v>1</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16" t="b">
         <v>0</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" s="1" t="n"/>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>3-1</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A16:A17"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1097,22 +1115,22 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>210.000</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>15.000</t>
+          <t>145.000</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>+90.91%</t>
+          <t>-100.00%</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>-86.36%</t>
+          <t>+31.82%</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>

</xml_diff>